<commit_message>
add missing qids to nel gold
</commit_message>
<xml_diff>
--- a/gold_standard/gold/nel_gold.xlsx
+++ b/gold_standard/gold/nel_gold.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssariter/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathankarr/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67B905EC-7310-994A-84AD-2DD4109E5A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E7FE55-D5C4-5845-8F1B-98B8BB7CD0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="909">
   <si>
     <t>index</t>
   </si>
@@ -2751,13 +2751,25 @@
   </si>
   <si>
     <t>AILERON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-23) MR. TIMOTHY ALLEN WELLS WAS ACTING AS PILOT IN COMMAND OF A BELL HELICOPTER MODEL BHT-47-G5, N4754R, ENGAGED </t>
+  </si>
+  <si>
+    <t>20000215010329A</t>
+  </si>
+  <si>
+    <t>PILOT TAXIED INTO UNMARKED DITCH AT END OF TAXIWAY.</t>
+  </si>
+  <si>
+    <t>19781113027039I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2833,6 +2845,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2889,7 +2907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2913,6 +2931,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3132,7 +3151,7 @@
   <dimension ref="A1:G1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3464,9 +3483,7 @@
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>1024</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="D25" s="3" t="s">
         <v>46</v>
       </c>
@@ -3478,9 +3495,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <v>1024</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="D26" s="3" t="s">
         <v>57</v>
       </c>
@@ -3492,9 +3507,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
-        <v>1024</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="C27" s="7"/>
       <c r="D27" s="3" t="s">
         <v>59</v>
@@ -3505,6 +3518,12 @@
       <c r="A28" s="3">
         <v>2335</v>
       </c>
+      <c r="B28" s="17" t="s">
+        <v>906</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>905</v>
+      </c>
       <c r="D28" s="3" t="s">
         <v>60</v>
       </c>
@@ -3517,9 +3536,7 @@
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>2335</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="D29" s="3" t="s">
         <v>63</v>
       </c>
@@ -3531,9 +3548,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>2335</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="D30" s="3" t="s">
         <v>65</v>
       </c>
@@ -3545,9 +3560,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>2335</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="D31" s="3" t="s">
         <v>34</v>
       </c>
@@ -3559,9 +3572,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>2335</v>
-      </c>
+      <c r="A32" s="3"/>
       <c r="D32" s="3" t="s">
         <v>67</v>
       </c>
@@ -3569,9 +3580,7 @@
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
-        <v>2335</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>68</v>
       </c>
@@ -5234,6 +5243,12 @@
       <c r="F171" s="3"/>
     </row>
     <row r="172" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B172" s="17" t="s">
+        <v>908</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>907</v>
+      </c>
       <c r="D172" s="3" t="s">
         <v>63</v>
       </c>

</xml_diff>